<commit_message>
Updated tests to ensure success test
</commit_message>
<xml_diff>
--- a/test/DATA/test_parametric_runs/Scenarios.xlsx
+++ b/test/DATA/test_parametric_runs/Scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eneait-my.sharepoint.com/personal/francesco_baldi_enea_it/Documents/Documents/Software/OptiENEA_github/OptiENEA/test/DATA/test_parametric_runs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="8_{ADE25E99-278E-41B7-BBB0-C156F4F6843B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DFF7DD1-652B-4A2D-BE20-9ACA04C7B611}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{ADE25E99-278E-41B7-BBB0-C156F4F6843B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3E87664-4E37-4C56-9A0B-26A3B202FC42}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -422,20 +422,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -452,7 +451,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -469,7 +468,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -486,7 +485,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -503,7 +502,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -520,7 +519,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -537,7 +536,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -554,7 +553,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -580,16 +579,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F15D9ED-30BC-4DE9-BA78-9DCEACC461AA}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>16</v>
       </c>
@@ -597,7 +596,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -608,7 +607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -619,7 +618,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -630,7 +629,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -641,7 +640,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>

</xml_diff>